<commit_message>
cambios en el cp4
</commit_message>
<xml_diff>
--- a/Test_cases/Caso de prueba 4.xlsx
+++ b/Test_cases/Caso de prueba 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lautaroacosta/Documents/Facultad/Testing/Grupo0102/Test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B5E7A5-07F9-9044-BF2C-ADCD02AC9525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8240D55A-64DD-6B46-95FE-474A16CE8A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="500" windowWidth="30220" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="500" windowWidth="28460" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>PE-44</t>
+  </si>
+  <si>
+    <t>Lautaro Acosta</t>
   </si>
 </sst>
 </file>
@@ -683,6 +686,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -694,9 +706,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,30 +730,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,8 +952,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="181" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:E43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -969,12 +972,12 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -994,10 +997,12 @@
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1050,7 +1055,7 @@
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -1084,8 +1089,8 @@
       <c r="E6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1109,8 +1114,8 @@
       <c r="E7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1130,8 +1135,8 @@
       <c r="C8" s="4"/>
       <c r="D8" s="13"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1151,8 +1156,8 @@
       <c r="C9" s="4"/>
       <c r="D9" s="13"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1172,8 +1177,8 @@
       <c r="C10" s="4"/>
       <c r="D10" s="13"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1206,8 +1211,8 @@
       <c r="C12" s="4"/>
       <c r="D12" s="13"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1241,16 +1246,16 @@
       <c r="D14" s="13"/>
       <c r="E14" s="4"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="58"/>
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1260,22 +1265,22 @@
       <c r="D15" s="13"/>
       <c r="E15" s="4"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="50"/>
-      <c r="I15" s="51" t="s">
+      <c r="H15" s="58"/>
+      <c r="I15" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="50"/>
-      <c r="K15" s="51" t="s">
+      <c r="J15" s="58"/>
+      <c r="K15" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="50"/>
-      <c r="M15" s="51" t="s">
+      <c r="L15" s="58"/>
+      <c r="M15" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="50"/>
+      <c r="N15" s="58"/>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1285,22 +1290,22 @@
       <c r="D16" s="13"/>
       <c r="E16" s="4"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="51" t="s">
+      <c r="G16" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51" t="s">
+      <c r="H16" s="58"/>
+      <c r="I16" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="51" t="s">
+      <c r="J16" s="58"/>
+      <c r="K16" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="50"/>
-      <c r="M16" s="51" t="s">
+      <c r="L16" s="58"/>
+      <c r="M16" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="50"/>
+      <c r="N16" s="58"/>
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1399,15 +1404,15 @@
       <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="17"/>
       <c r="G20" s="27" t="s">
         <v>31</v>
@@ -1434,11 +1439,11 @@
       <c r="O20" s="4"/>
     </row>
     <row r="21" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="39"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="37"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1496,14 +1501,14 @@
       <c r="A24" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="52" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="53"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1519,14 +1524,14 @@
       <c r="A25" s="35">
         <v>1</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="57" t="s">
+      <c r="C25" s="49"/>
+      <c r="D25" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="53"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1538,18 +1543,18 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="35">
         <v>2</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="59" t="s">
+      <c r="C26" s="49"/>
+      <c r="D26" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="60"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1565,14 +1570,14 @@
       <c r="A27" s="35">
         <v>3</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="59" t="s">
+      <c r="C27" s="49"/>
+      <c r="D27" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="60"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="4"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
@@ -1588,114 +1593,114 @@
       <c r="A28" s="13"/>
       <c r="B28" s="54"/>
       <c r="C28" s="55"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="56" t="s">
+      <c r="G28" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="53"/>
-      <c r="I28" s="56" t="s">
+      <c r="H28" s="49"/>
+      <c r="I28" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="53"/>
-      <c r="K28" s="56" t="s">
+      <c r="J28" s="49"/>
+      <c r="K28" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L28" s="53"/>
-      <c r="M28" s="56" t="s">
+      <c r="L28" s="49"/>
+      <c r="M28" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="53"/>
+      <c r="N28" s="49"/>
       <c r="O28" s="4"/>
     </row>
     <row r="29" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="13"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="37"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="40"/>
       <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="13"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="37"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="40"/>
       <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="13"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
       <c r="F31" s="17"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="37"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="40"/>
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="17"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="37"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="40"/>
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="39"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="37"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="40"/>
       <c r="F33" s="17"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="37"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="40"/>
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.2">
@@ -1744,14 +1749,14 @@
       <c r="A36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="52" t="s">
+      <c r="C36" s="49"/>
+      <c r="D36" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="53"/>
+      <c r="E36" s="49"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -1767,14 +1772,14 @@
       <c r="A37" s="35">
         <v>1</v>
       </c>
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="59" t="s">
+      <c r="C37" s="49"/>
+      <c r="D37" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="60"/>
+      <c r="E37" s="38"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -1786,18 +1791,18 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="35">
         <v>2</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="59" t="s">
+      <c r="C38" s="49"/>
+      <c r="D38" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="60"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -1813,14 +1818,14 @@
       <c r="A39" s="35">
         <v>3</v>
       </c>
-      <c r="B39" s="57" t="s">
+      <c r="B39" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="59" t="s">
+      <c r="C39" s="49"/>
+      <c r="D39" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="38"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -1832,18 +1837,18 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="35">
         <v>4</v>
       </c>
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="D40" s="59" t="s">
+      <c r="C40" s="49"/>
+      <c r="D40" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="60"/>
+      <c r="E40" s="38"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -1859,14 +1864,14 @@
       <c r="A41" s="35">
         <v>5</v>
       </c>
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="59" t="s">
+      <c r="C41" s="49"/>
+      <c r="D41" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="60"/>
+      <c r="E41" s="38"/>
       <c r="F41" s="4"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -1880,46 +1885,46 @@
     </row>
     <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="35"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="37"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="56" t="s">
+      <c r="G42" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H42" s="53"/>
-      <c r="I42" s="56" t="s">
+      <c r="H42" s="49"/>
+      <c r="I42" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="J42" s="53"/>
-      <c r="K42" s="56" t="s">
+      <c r="J42" s="49"/>
+      <c r="K42" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L42" s="53"/>
-      <c r="M42" s="56" t="s">
+      <c r="L42" s="49"/>
+      <c r="M42" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="N42" s="53"/>
+      <c r="N42" s="49"/>
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="1:15" ht="14" x14ac:dyDescent="0.2">
       <c r="A43" s="35"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="37"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="58" t="s">
+      <c r="G43" s="39"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="J43" s="53"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="37"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="40"/>
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -1929,52 +1934,52 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="37"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="40"/>
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="42"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="45"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="37"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="37"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="40"/>
       <c r="O45" s="4"/>
     </row>
     <row r="46" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="39"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="37"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="40"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="37"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="37"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="40"/>
       <c r="O46" s="4"/>
     </row>
     <row r="47" spans="1:15" ht="15" x14ac:dyDescent="0.2">
@@ -1992,14 +1997,14 @@
         <v>39</v>
       </c>
       <c r="F47" s="4"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="37"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="37"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="40"/>
       <c r="O47" s="4"/>
     </row>
     <row r="48" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -2023,14 +2028,14 @@
       <c r="A49" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="53"/>
-      <c r="D49" s="52" t="s">
+      <c r="C49" s="49"/>
+      <c r="D49" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="53"/>
+      <c r="E49" s="49"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -2046,14 +2051,14 @@
       <c r="A50" s="35">
         <v>1</v>
       </c>
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="53"/>
-      <c r="D50" s="59" t="s">
+      <c r="C50" s="49"/>
+      <c r="D50" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="60"/>
+      <c r="E50" s="38"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -2065,18 +2070,18 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
     </row>
-    <row r="51" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="35">
         <v>2</v>
       </c>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="53"/>
-      <c r="D51" s="59" t="s">
+      <c r="C51" s="49"/>
+      <c r="D51" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E51" s="60"/>
+      <c r="E51" s="38"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -2088,18 +2093,18 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
     </row>
-    <row r="52" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" ht="47" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="35">
         <v>3</v>
       </c>
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="53"/>
-      <c r="D52" s="59" t="s">
+      <c r="C52" s="49"/>
+      <c r="D52" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="60"/>
+      <c r="E52" s="38"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -2115,14 +2120,14 @@
       <c r="A53" s="35">
         <v>4</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="59" t="s">
+      <c r="C53" s="49"/>
+      <c r="D53" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E53" s="60"/>
+      <c r="E53" s="38"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -2138,14 +2143,14 @@
       <c r="A54" s="35">
         <v>5</v>
       </c>
-      <c r="B54" s="57" t="s">
+      <c r="B54" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="53"/>
-      <c r="D54" s="59" t="s">
+      <c r="C54" s="49"/>
+      <c r="D54" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="60"/>
+      <c r="E54" s="38"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -2159,36 +2164,68 @@
     </row>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:E46"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:E33"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:E21"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="B37:C37"/>
@@ -2213,68 +2250,36 @@
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:E21"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:E33"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:E46"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="M46:N46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>